<commit_message>
Added BAU scenario .cin name
</commit_message>
<xml_diff>
--- a/WebAppData.xlsx
+++ b/WebAppData.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23426"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox (Energy Innovation)\EI-PlcyMdl\eps-2.0.0-saudiarabia-wipH\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rorvis\Dropbox (Energy InNovation)\My Documents\Energy Policy Solutions\Saudi Arabia\Models\eps-saudiarabia\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90158A2A-603B-44A9-BEEF-BC72AD61108A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="435" windowWidth="18960" windowHeight="6210"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="10" r:id="rId1"/>
@@ -23,17 +24,28 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">PolicyLevers!$A$1:$P$535</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Jeffrey Rissman</author>
   </authors>
   <commentList>
-    <comment ref="K200" authorId="0" shapeId="0">
+    <comment ref="K200" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000001000000}">
       <text>
         <r>
           <rPr>
@@ -57,7 +69,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K201" authorId="0" shapeId="0">
+    <comment ref="K201" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000002000000}">
       <text>
         <r>
           <rPr>
@@ -81,7 +93,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K202" authorId="0" shapeId="0">
+    <comment ref="K202" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000003000000}">
       <text>
         <r>
           <rPr>
@@ -105,7 +117,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K203" authorId="0" shapeId="0">
+    <comment ref="K203" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000004000000}">
       <text>
         <r>
           <rPr>
@@ -129,7 +141,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K204" authorId="0" shapeId="0">
+    <comment ref="K204" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000005000000}">
       <text>
         <r>
           <rPr>
@@ -153,7 +165,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K205" authorId="0" shapeId="0">
+    <comment ref="K205" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000006000000}">
       <text>
         <r>
           <rPr>
@@ -177,7 +189,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K206" authorId="0" shapeId="0">
+    <comment ref="K206" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000007000000}">
       <text>
         <r>
           <rPr>
@@ -201,7 +213,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K208" authorId="0" shapeId="0">
+    <comment ref="K208" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000008000000}">
       <text>
         <r>
           <rPr>
@@ -225,7 +237,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K209" authorId="0" shapeId="0">
+    <comment ref="K209" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000009000000}">
       <text>
         <r>
           <rPr>
@@ -249,7 +261,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K210" authorId="0" shapeId="0">
+    <comment ref="K210" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-00000A000000}">
       <text>
         <r>
           <rPr>
@@ -273,7 +285,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K211" authorId="0" shapeId="0">
+    <comment ref="K211" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-00000B000000}">
       <text>
         <r>
           <rPr>
@@ -297,7 +309,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K212" authorId="0" shapeId="0">
+    <comment ref="K212" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-00000C000000}">
       <text>
         <r>
           <rPr>
@@ -321,7 +333,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K213" authorId="0" shapeId="0">
+    <comment ref="K213" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-00000D000000}">
       <text>
         <r>
           <rPr>
@@ -345,7 +357,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K214" authorId="0" shapeId="0">
+    <comment ref="K214" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-00000E000000}">
       <text>
         <r>
           <rPr>
@@ -369,7 +381,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K215" authorId="0" shapeId="0">
+    <comment ref="K215" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-00000F000000}">
       <text>
         <r>
           <rPr>
@@ -393,7 +405,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K216" authorId="0" shapeId="0">
+    <comment ref="K216" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000010000000}">
       <text>
         <r>
           <rPr>
@@ -417,7 +429,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K218" authorId="0" shapeId="0">
+    <comment ref="K218" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000011000000}">
       <text>
         <r>
           <rPr>
@@ -446,18 +458,18 @@
 </file>
 
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
-<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <connection id="1" name="OuputGraphSchema" type="4" refreshedVersion="0" background="1">
+<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16">
+  <connection id="1" xr16:uid="{00000000-0015-0000-FFFF-FFFF00000000}" name="OuputGraphSchema" type="4" refreshedVersion="0" background="1">
     <webPr xml="1" sourceData="1" url="Z:\todd\Projects\PolicySolutions\tools\lib\OuputGraphSchema.xml" htmlTables="1" htmlFormat="all"/>
   </connection>
-  <connection id="2" name="PolicyLeverSchema" type="4" refreshedVersion="0" background="1">
+  <connection id="2" xr16:uid="{00000000-0015-0000-FFFF-FFFF01000000}" name="PolicyLeverSchema" type="4" refreshedVersion="0" background="1">
     <webPr xml="1" sourceData="1" url="Z:\todd\Projects\PolicySolutions\tools\lib\PolicyLeverSchema.xml" htmlTables="1" htmlFormat="all"/>
   </connection>
 </connections>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4786" uniqueCount="1578">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4786" uniqueCount="1579">
   <si>
     <t>Short Name</t>
   </si>
@@ -5477,11 +5489,14 @@
   <si>
     <t>Output Water Consumed by Power Plants[geothermal es]; Output Water Consumed by Power Plants[solar thermal es]; Output Water Consumed by Power Plants[solar PV es]; Output Water Consumed by Power Plants[nuclear es]; Output Water Consumed by Power Plants[municipal solid waste es]; Output Water Consumed by Power Plants[petroleum es]; Output Water Consumed by Power Plants[heavy or residual fuel oil es]; Output Water Consumed by Power Plants[crude oil es]; Output Water Consumed by Power Plants[natural gas peaker es]; Output Water Consumed by Power Plants[natural gas nonpeaker es]</t>
   </si>
+  <si>
+    <t>Scenario_BAU.cin</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="5">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="0.0%"/>
@@ -6679,6 +6694,9 @@
     <xf numFmtId="1" fontId="0" fillId="30" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="13" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -6688,34 +6706,31 @@
     <xf numFmtId="0" fontId="13" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="20">
-    <cellStyle name="2x indented GHG Textfiels" xfId="10"/>
-    <cellStyle name="5x indented GHG Textfiels" xfId="11"/>
-    <cellStyle name="AggCels" xfId="12"/>
-    <cellStyle name="AggGreen_bld" xfId="15"/>
-    <cellStyle name="Body: normal cell 2" xfId="5"/>
-    <cellStyle name="Comma 6" xfId="6"/>
-    <cellStyle name="Constants" xfId="8"/>
-    <cellStyle name="CustomizationCells" xfId="17"/>
-    <cellStyle name="Empty_B_border" xfId="16"/>
-    <cellStyle name="Header: bottom row 2" xfId="4"/>
-    <cellStyle name="Headline" xfId="7"/>
+    <cellStyle name="2x indented GHG Textfiels" xfId="10" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
+    <cellStyle name="5x indented GHG Textfiels" xfId="11" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="AggCels" xfId="12" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
+    <cellStyle name="AggGreen_bld" xfId="15" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
+    <cellStyle name="Body: normal cell 2" xfId="5" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
+    <cellStyle name="Comma 6" xfId="6" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
+    <cellStyle name="Constants" xfId="8" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
+    <cellStyle name="CustomizationCells" xfId="17" xr:uid="{00000000-0005-0000-0000-000007000000}"/>
+    <cellStyle name="Empty_B_border" xfId="16" xr:uid="{00000000-0005-0000-0000-000008000000}"/>
+    <cellStyle name="Header: bottom row 2" xfId="4" xr:uid="{00000000-0005-0000-0000-000009000000}"/>
+    <cellStyle name="Headline" xfId="7" xr:uid="{00000000-0005-0000-0000-00000A000000}"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
     <cellStyle name="Neutral" xfId="19" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="3"/>
-    <cellStyle name="Normal 3" xfId="18"/>
-    <cellStyle name="Normal GHG Textfiels Bold" xfId="9"/>
-    <cellStyle name="Normal GHG-Shade" xfId="14"/>
+    <cellStyle name="Normal 2" xfId="3" xr:uid="{00000000-0005-0000-0000-00000E000000}"/>
+    <cellStyle name="Normal 3" xfId="18" xr:uid="{00000000-0005-0000-0000-00000F000000}"/>
+    <cellStyle name="Normal GHG Textfiels Bold" xfId="9" xr:uid="{00000000-0005-0000-0000-000010000000}"/>
+    <cellStyle name="Normal GHG-Shade" xfId="14" xr:uid="{00000000-0005-0000-0000-000011000000}"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
-    <cellStyle name="Обычный_CRF2002 (1)" xfId="13"/>
+    <cellStyle name="Обычный_CRF2002 (1)" xfId="13" xr:uid="{00000000-0005-0000-0000-000013000000}"/>
   </cellStyles>
   <dxfs count="40">
     <dxf>
@@ -7663,10 +7678,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
@@ -7879,7 +7894,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A10" r:id="rId1"/>
+    <hyperlink ref="A10" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId2"/>
@@ -7887,7 +7902,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:T560"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
@@ -38934,185 +38949,57 @@
       <c r="R544" s="4"/>
       <c r="T544" s="4"/>
     </row>
-    <row r="545" spans="1:20">
-      <c r="A545" s="4"/>
-      <c r="B545" s="4"/>
-      <c r="C545" s="4"/>
-      <c r="H545" s="4"/>
-      <c r="J545" s="4"/>
-      <c r="M545" s="4"/>
-      <c r="N545" s="4"/>
-      <c r="R545" s="4"/>
-      <c r="T545" s="4"/>
-    </row>
-    <row r="546" spans="1:20">
-      <c r="A546" s="4"/>
-      <c r="B546" s="4"/>
-      <c r="C546" s="4"/>
-      <c r="H546" s="4"/>
-      <c r="J546" s="4"/>
-      <c r="M546" s="4"/>
-      <c r="N546" s="4"/>
-      <c r="R546" s="4"/>
-      <c r="T546" s="4"/>
-    </row>
-    <row r="547" spans="1:20">
-      <c r="A547" s="4"/>
-      <c r="B547" s="4"/>
-      <c r="C547" s="4"/>
-      <c r="H547" s="4"/>
+    <row r="545" spans="9:19" s="4" customFormat="1">
+      <c r="S545" s="6"/>
+    </row>
+    <row r="546" spans="9:19" s="4" customFormat="1">
+      <c r="S546" s="6"/>
+    </row>
+    <row r="547" spans="9:19" s="4" customFormat="1">
       <c r="I547" s="52"/>
-      <c r="J547" s="4"/>
-      <c r="M547" s="4"/>
-      <c r="N547" s="4"/>
-      <c r="R547" s="4"/>
-      <c r="T547" s="4"/>
-    </row>
-    <row r="548" spans="1:20">
-      <c r="A548" s="4"/>
-      <c r="B548" s="4"/>
-      <c r="C548" s="4"/>
-      <c r="H548" s="4"/>
-      <c r="J548" s="4"/>
-      <c r="M548" s="4"/>
-      <c r="N548" s="4"/>
-      <c r="R548" s="4"/>
-      <c r="T548" s="4"/>
-    </row>
-    <row r="549" spans="1:20">
-      <c r="A549" s="4"/>
-      <c r="B549" s="4"/>
-      <c r="C549" s="4"/>
-      <c r="H549" s="4"/>
-      <c r="J549" s="4"/>
-      <c r="M549" s="4"/>
-      <c r="N549" s="4"/>
-      <c r="R549" s="4"/>
-      <c r="T549" s="4"/>
-    </row>
-    <row r="550" spans="1:20">
-      <c r="A550" s="4"/>
-      <c r="B550" s="4"/>
-      <c r="C550" s="4"/>
-      <c r="H550" s="4"/>
-      <c r="J550" s="4"/>
-      <c r="M550" s="4"/>
-      <c r="N550" s="4"/>
-      <c r="R550" s="4"/>
-      <c r="T550" s="4"/>
-    </row>
-    <row r="551" spans="1:20">
-      <c r="A551" s="4"/>
-      <c r="B551" s="4"/>
-      <c r="C551" s="4"/>
-      <c r="H551" s="4"/>
-      <c r="J551" s="4"/>
-      <c r="M551" s="4"/>
-      <c r="N551" s="4"/>
-      <c r="R551" s="4"/>
-      <c r="T551" s="4"/>
-    </row>
-    <row r="552" spans="1:20">
-      <c r="A552" s="4"/>
-      <c r="B552" s="4"/>
-      <c r="C552" s="4"/>
-      <c r="H552" s="4"/>
-      <c r="J552" s="4"/>
-      <c r="M552" s="4"/>
-      <c r="N552" s="4"/>
-      <c r="R552" s="4"/>
-      <c r="T552" s="4"/>
-    </row>
-    <row r="553" spans="1:20">
-      <c r="A553" s="4"/>
-      <c r="B553" s="4"/>
-      <c r="C553" s="4"/>
-      <c r="H553" s="4"/>
-      <c r="J553" s="4"/>
-      <c r="M553" s="4"/>
-      <c r="N553" s="4"/>
-      <c r="R553" s="4"/>
-      <c r="T553" s="4"/>
-    </row>
-    <row r="554" spans="1:20">
-      <c r="A554" s="4"/>
-      <c r="B554" s="4"/>
-      <c r="C554" s="4"/>
-      <c r="H554" s="4"/>
-      <c r="J554" s="4"/>
-      <c r="M554" s="4"/>
-      <c r="N554" s="4"/>
-      <c r="R554" s="4"/>
-      <c r="T554" s="4"/>
-    </row>
-    <row r="555" spans="1:20">
-      <c r="A555" s="4"/>
-      <c r="B555" s="4"/>
-      <c r="C555" s="4"/>
-      <c r="H555" s="4"/>
-      <c r="J555" s="4"/>
-      <c r="M555" s="4"/>
-      <c r="N555" s="4"/>
-      <c r="R555" s="4"/>
-      <c r="T555" s="4"/>
-    </row>
-    <row r="556" spans="1:20">
-      <c r="A556" s="4"/>
-      <c r="B556" s="4"/>
-      <c r="C556" s="4"/>
-      <c r="H556" s="4"/>
-      <c r="J556" s="4"/>
-      <c r="M556" s="4"/>
-      <c r="N556" s="4"/>
-      <c r="R556" s="4"/>
-      <c r="T556" s="4"/>
-    </row>
-    <row r="557" spans="1:20">
-      <c r="A557" s="4"/>
-      <c r="B557" s="4"/>
-      <c r="C557" s="4"/>
-      <c r="H557" s="4"/>
-      <c r="J557" s="4"/>
-      <c r="M557" s="4"/>
-      <c r="N557" s="4"/>
-      <c r="R557" s="4"/>
-      <c r="T557" s="4"/>
-    </row>
-    <row r="558" spans="1:20">
-      <c r="A558" s="4"/>
-      <c r="B558" s="4"/>
-      <c r="C558" s="4"/>
-      <c r="H558" s="4"/>
-      <c r="J558" s="4"/>
-      <c r="M558" s="4"/>
-      <c r="N558" s="4"/>
-      <c r="R558" s="4"/>
-      <c r="T558" s="4"/>
-    </row>
-    <row r="559" spans="1:20">
-      <c r="A559" s="4"/>
-      <c r="B559" s="4"/>
-      <c r="C559" s="4"/>
-      <c r="H559" s="4"/>
-      <c r="J559" s="4"/>
-      <c r="M559" s="4"/>
-      <c r="N559" s="4"/>
-      <c r="R559" s="4"/>
-      <c r="T559" s="4"/>
-    </row>
-    <row r="560" spans="1:20">
-      <c r="A560" s="4"/>
-      <c r="B560" s="4"/>
-      <c r="C560" s="4"/>
-      <c r="H560" s="4"/>
-      <c r="J560" s="4"/>
-      <c r="M560" s="4"/>
-      <c r="N560" s="4"/>
-      <c r="R560" s="4"/>
-      <c r="T560" s="4"/>
+      <c r="S547" s="6"/>
+    </row>
+    <row r="548" spans="9:19" s="4" customFormat="1">
+      <c r="S548" s="6"/>
+    </row>
+    <row r="549" spans="9:19" s="4" customFormat="1">
+      <c r="S549" s="6"/>
+    </row>
+    <row r="550" spans="9:19" s="4" customFormat="1">
+      <c r="S550" s="6"/>
+    </row>
+    <row r="551" spans="9:19" s="4" customFormat="1">
+      <c r="S551" s="6"/>
+    </row>
+    <row r="552" spans="9:19" s="4" customFormat="1">
+      <c r="S552" s="6"/>
+    </row>
+    <row r="553" spans="9:19" s="4" customFormat="1">
+      <c r="S553" s="6"/>
+    </row>
+    <row r="554" spans="9:19" s="4" customFormat="1">
+      <c r="S554" s="6"/>
+    </row>
+    <row r="555" spans="9:19" s="4" customFormat="1">
+      <c r="S555" s="6"/>
+    </row>
+    <row r="556" spans="9:19" s="4" customFormat="1">
+      <c r="S556" s="6"/>
+    </row>
+    <row r="557" spans="9:19" s="4" customFormat="1">
+      <c r="S557" s="6"/>
+    </row>
+    <row r="558" spans="9:19" s="4" customFormat="1">
+      <c r="S558" s="6"/>
+    </row>
+    <row r="559" spans="9:19" s="4" customFormat="1">
+      <c r="S559" s="6"/>
+    </row>
+    <row r="560" spans="9:19" s="4" customFormat="1">
+      <c r="S560" s="6"/>
     </row>
   </sheetData>
-  <sortState ref="A119:I139">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A119:I139">
     <sortCondition ref="B119:B139"/>
   </sortState>
   <conditionalFormatting sqref="I76:I88 I487:I488 I522 I527:I546 I548:I1048576 I90:I99 I1:I9 I12:I19 I24 I33:I36 I43:I46 I53:I59 I38:I39 I48:I49 I63:I64 I113:I176 I492:I520 I373:I485 I178:I302">
@@ -39316,8 +39203,8 @@
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="T390" r:id="rId1" display="https://www.fas.org/sgp/crs/misc/R40562.pdf, p.3, paragraph 1"/>
-    <hyperlink ref="S101" r:id="rId2"/>
+    <hyperlink ref="T390" r:id="rId1" display="https://www.fas.org/sgp/crs/misc/R40562.pdf, p.3, paragraph 1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
+    <hyperlink ref="S101" r:id="rId2" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId3"/>
@@ -39329,7 +39216,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:H119"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
@@ -42226,7 +42113,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr>
     <tabColor theme="9"/>
   </sheetPr>
@@ -44344,10 +44231,12 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
@@ -44369,7 +44258,7 @@
         <v>158</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>81</v>
+        <v>1578</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -44395,7 +44284,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -44488,7 +44377,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A15" r:id="rId1"/>
+    <hyperlink ref="A15" r:id="rId1" xr:uid="{00000000-0004-0000-0500-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>
@@ -44496,7 +44385,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:AM197"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
@@ -44526,13 +44415,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" s="198" t="s">
+      <c r="A1" s="195" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="198"/>
-      <c r="C1" s="198"/>
-      <c r="D1" s="198"/>
-      <c r="E1" s="198"/>
+      <c r="B1" s="195"/>
+      <c r="C1" s="195"/>
+      <c r="D1" s="195"/>
+      <c r="E1" s="195"/>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="199" t="s">
@@ -44601,13 +44490,13 @@
       </c>
     </row>
     <row r="60" spans="1:5">
-      <c r="A60" s="198" t="s">
+      <c r="A60" s="195" t="s">
         <v>181</v>
       </c>
-      <c r="B60" s="198"/>
-      <c r="C60" s="198"/>
-      <c r="D60" s="198"/>
-      <c r="E60" s="198"/>
+      <c r="B60" s="195"/>
+      <c r="C60" s="195"/>
+      <c r="D60" s="195"/>
+      <c r="E60" s="195"/>
     </row>
     <row r="85" spans="1:39" s="12" customFormat="1">
       <c r="A85" s="9" t="s">
@@ -44712,13 +44601,13 @@
       </c>
     </row>
     <row r="89" spans="1:39">
-      <c r="A89" s="198" t="s">
+      <c r="A89" s="195" t="s">
         <v>182</v>
       </c>
-      <c r="B89" s="198"/>
-      <c r="C89" s="198"/>
-      <c r="D89" s="198"/>
-      <c r="E89" s="198"/>
+      <c r="B89" s="195"/>
+      <c r="C89" s="195"/>
+      <c r="D89" s="195"/>
+      <c r="E89" s="195"/>
     </row>
     <row r="90" spans="1:39">
       <c r="A90" s="9">
@@ -44805,13 +44694,13 @@
       </c>
     </row>
     <row r="98" spans="1:5">
-      <c r="A98" s="198" t="s">
+      <c r="A98" s="195" t="s">
         <v>183</v>
       </c>
-      <c r="B98" s="198"/>
-      <c r="C98" s="198"/>
-      <c r="D98" s="198"/>
-      <c r="E98" s="198"/>
+      <c r="B98" s="195"/>
+      <c r="C98" s="195"/>
+      <c r="D98" s="195"/>
+      <c r="E98" s="195"/>
     </row>
     <row r="99" spans="1:5">
       <c r="A99" s="17">
@@ -44895,13 +44784,13 @@
       <c r="A108" s="20"/>
     </row>
     <row r="109" spans="1:5">
-      <c r="A109" s="198" t="s">
+      <c r="A109" s="195" t="s">
         <v>185</v>
       </c>
-      <c r="B109" s="198"/>
-      <c r="C109" s="198"/>
-      <c r="D109" s="198"/>
-      <c r="E109" s="198"/>
+      <c r="B109" s="195"/>
+      <c r="C109" s="195"/>
+      <c r="D109" s="195"/>
+      <c r="E109" s="195"/>
     </row>
     <row r="110" spans="1:5" ht="15.75" thickBot="1"/>
     <row r="111" spans="1:5" ht="15.75" thickBot="1">
@@ -44914,13 +44803,13 @@
       </c>
     </row>
     <row r="113" spans="1:14">
-      <c r="A113" s="198" t="s">
+      <c r="A113" s="195" t="s">
         <v>184</v>
       </c>
-      <c r="B113" s="198"/>
-      <c r="C113" s="198"/>
-      <c r="D113" s="198"/>
-      <c r="E113" s="198"/>
+      <c r="B113" s="195"/>
+      <c r="C113" s="195"/>
+      <c r="D113" s="195"/>
+      <c r="E113" s="195"/>
     </row>
     <row r="114" spans="1:14">
       <c r="A114" s="17">
@@ -45001,13 +44890,13 @@
       </c>
     </row>
     <row r="124" spans="1:14">
-      <c r="A124" s="198" t="s">
+      <c r="A124" s="195" t="s">
         <v>450</v>
       </c>
-      <c r="B124" s="198"/>
-      <c r="C124" s="198"/>
-      <c r="D124" s="198"/>
-      <c r="E124" s="198"/>
+      <c r="B124" s="195"/>
+      <c r="C124" s="195"/>
+      <c r="D124" s="195"/>
+      <c r="E124" s="195"/>
       <c r="L124" s="21"/>
     </row>
     <row r="125" spans="1:14">
@@ -45098,13 +44987,13 @@
       <c r="C133" s="15"/>
     </row>
     <row r="134" spans="1:14">
-      <c r="A134" s="198" t="s">
+      <c r="A134" s="195" t="s">
         <v>110</v>
       </c>
-      <c r="B134" s="198"/>
-      <c r="C134" s="198"/>
-      <c r="D134" s="198"/>
-      <c r="E134" s="198"/>
+      <c r="B134" s="195"/>
+      <c r="C134" s="195"/>
+      <c r="D134" s="195"/>
+      <c r="E134" s="195"/>
     </row>
     <row r="135" spans="1:14">
       <c r="A135" s="27" t="s">
@@ -45119,25 +45008,25 @@
     </row>
     <row r="136" spans="1:14" ht="15.75">
       <c r="A136" s="29"/>
-      <c r="B136" s="195" t="s">
+      <c r="B136" s="196" t="s">
         <v>470</v>
       </c>
-      <c r="C136" s="196"/>
-      <c r="D136" s="196"/>
-      <c r="E136" s="197"/>
+      <c r="C136" s="197"/>
+      <c r="D136" s="197"/>
+      <c r="E136" s="198"/>
       <c r="F136" s="28"/>
       <c r="G136" s="28"/>
     </row>
     <row r="137" spans="1:14" ht="15.75">
       <c r="A137" s="30"/>
-      <c r="B137" s="195" t="s">
+      <c r="B137" s="196" t="s">
         <v>471</v>
       </c>
-      <c r="C137" s="197"/>
-      <c r="D137" s="195" t="s">
+      <c r="C137" s="198"/>
+      <c r="D137" s="196" t="s">
         <v>472</v>
       </c>
-      <c r="E137" s="197"/>
+      <c r="E137" s="198"/>
       <c r="F137" s="28"/>
       <c r="G137" s="28"/>
     </row>
@@ -45684,13 +45573,13 @@
       <c r="G163" s="28"/>
     </row>
     <row r="165" spans="1:7">
-      <c r="A165" s="198" t="s">
+      <c r="A165" s="195" t="s">
         <v>188</v>
       </c>
-      <c r="B165" s="198"/>
-      <c r="C165" s="198"/>
-      <c r="D165" s="198"/>
-      <c r="E165" s="198"/>
+      <c r="B165" s="195"/>
+      <c r="C165" s="195"/>
+      <c r="D165" s="195"/>
+      <c r="E165" s="195"/>
     </row>
     <row r="166" spans="1:7" ht="15.75" thickBot="1">
       <c r="A166" s="23" t="s">
@@ -45713,10 +45602,10 @@
       <c r="B168" s="46"/>
     </row>
     <row r="169" spans="1:7">
-      <c r="A169" s="198" t="s">
+      <c r="A169" s="195" t="s">
         <v>458</v>
       </c>
-      <c r="B169" s="198"/>
+      <c r="B169" s="195"/>
     </row>
     <row r="170" spans="1:7">
       <c r="A170" s="23" t="s">
@@ -45748,13 +45637,13 @@
       <c r="B173" s="46"/>
     </row>
     <row r="174" spans="1:7">
-      <c r="A174" s="198" t="s">
+      <c r="A174" s="195" t="s">
         <v>197</v>
       </c>
-      <c r="B174" s="198"/>
-      <c r="C174" s="198"/>
-      <c r="D174" s="198"/>
-      <c r="E174" s="198"/>
+      <c r="B174" s="195"/>
+      <c r="C174" s="195"/>
+      <c r="D174" s="195"/>
+      <c r="E174" s="195"/>
     </row>
     <row r="175" spans="1:7" ht="15.75" thickBot="1">
       <c r="A175" s="23" t="s">
@@ -45774,13 +45663,13 @@
       </c>
     </row>
     <row r="178" spans="1:5">
-      <c r="A178" s="198" t="s">
+      <c r="A178" s="195" t="s">
         <v>191</v>
       </c>
-      <c r="B178" s="198"/>
-      <c r="C178" s="198"/>
-      <c r="D178" s="198"/>
-      <c r="E178" s="198"/>
+      <c r="B178" s="195"/>
+      <c r="C178" s="195"/>
+      <c r="D178" s="195"/>
+      <c r="E178" s="195"/>
     </row>
     <row r="179" spans="1:5">
       <c r="A179" s="25" t="s">
@@ -45808,13 +45697,13 @@
       </c>
     </row>
     <row r="183" spans="1:5">
-      <c r="A183" s="198" t="s">
+      <c r="A183" s="195" t="s">
         <v>193</v>
       </c>
-      <c r="B183" s="198"/>
-      <c r="C183" s="198"/>
-      <c r="D183" s="198"/>
-      <c r="E183" s="198"/>
+      <c r="B183" s="195"/>
+      <c r="C183" s="195"/>
+      <c r="D183" s="195"/>
+      <c r="E183" s="195"/>
     </row>
     <row r="184" spans="1:5">
       <c r="A184" s="23" t="s">
@@ -45869,13 +45758,13 @@
       </c>
     </row>
     <row r="191" spans="1:5">
-      <c r="A191" s="198" t="s">
+      <c r="A191" s="195" t="s">
         <v>207</v>
       </c>
-      <c r="B191" s="198"/>
-      <c r="C191" s="198"/>
-      <c r="D191" s="198"/>
-      <c r="E191" s="198"/>
+      <c r="B191" s="195"/>
+      <c r="C191" s="195"/>
+      <c r="D191" s="195"/>
+      <c r="E191" s="195"/>
     </row>
     <row r="192" spans="1:5">
       <c r="A192" s="21" t="s">
@@ -45935,12 +45824,6 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="A191:E191"/>
-    <mergeCell ref="A165:E165"/>
-    <mergeCell ref="A178:E178"/>
-    <mergeCell ref="A183:E183"/>
-    <mergeCell ref="A174:E174"/>
-    <mergeCell ref="A169:B169"/>
     <mergeCell ref="B136:E136"/>
     <mergeCell ref="B137:C137"/>
     <mergeCell ref="D137:E137"/>
@@ -45955,6 +45838,12 @@
     <mergeCell ref="A113:E113"/>
     <mergeCell ref="A109:E109"/>
     <mergeCell ref="A124:E124"/>
+    <mergeCell ref="A191:E191"/>
+    <mergeCell ref="A165:E165"/>
+    <mergeCell ref="A178:E178"/>
+    <mergeCell ref="A183:E183"/>
+    <mergeCell ref="A174:E174"/>
+    <mergeCell ref="A169:B169"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Update to Short Name column in WebAppData file
</commit_message>
<xml_diff>
--- a/WebAppData.xlsx
+++ b/WebAppData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shelley\Dropbox (Energy Innovation)\PC (2)\Documents\GitHub_Repositories\eps-saudiarabia\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F4EF5B0-9E72-4AEF-A9D3-BB29EB701096}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{024082B1-B20D-49FD-A813-7F478CFE701B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -5152,220 +5152,220 @@
     <t>This tab contains information about each policy that does not vary by subscripted element of that policy.</t>
   </si>
   <si>
-    <t>Agriculture, Land Use, and Water- Desalination Energy Efficiency Standards</t>
-  </si>
-  <si>
-    <t>Agriculture, Land Use, and Water- Livestock Measures</t>
-  </si>
-  <si>
-    <t>Agriculture, Land Use, and Water- Rice Cultivation Measures</t>
-  </si>
-  <si>
-    <t>Agriculture, Land Use, and Water- Shift to Non-Animal Products</t>
-  </si>
-  <si>
-    <t>Agriculture, Land Use, and Water- Water Conservation</t>
-  </si>
-  <si>
-    <t>Buildings and Appliances- Building Component Electrification</t>
-  </si>
-  <si>
-    <t>Buildings and Appliances- Building Energy Efficiency Standards</t>
-  </si>
-  <si>
-    <t>Buildings and Appliances- Contractor Training</t>
-  </si>
-  <si>
-    <t>Buildings and Appliances- Distributed Solar Carve-Out</t>
-  </si>
-  <si>
-    <t>Buildings and Appliances- Distributed Solar Subsidy</t>
-  </si>
-  <si>
-    <t>Buildings and Appliances- Improved Labeling</t>
-  </si>
-  <si>
-    <t>Buildings and Appliances- Rebate for Efficient Products</t>
-  </si>
-  <si>
-    <t>Buildings and Appliances- Retrofit Existing Buildings</t>
-  </si>
-  <si>
-    <t>Cross-Sector- Domestic Carbon Pricing</t>
-  </si>
-  <si>
-    <t>Cross-Sector- Fuel Taxes</t>
-  </si>
-  <si>
-    <t>District Heat and Hydrogen- Switch District Heat Coal to NG</t>
-  </si>
-  <si>
-    <t>District Heat and Hydrogen- Use CHP for District Heat</t>
-  </si>
-  <si>
-    <t>Electricity Supply- Demand Response</t>
-  </si>
-  <si>
-    <t>Electricity Supply- Grid-Scale Electricity Storage</t>
-  </si>
-  <si>
-    <t>Electricity Supply- Increase Transmission</t>
-  </si>
-  <si>
-    <t>Electricity Supply- KSA 2030 Renewables Target</t>
-  </si>
-  <si>
-    <t>Electricity Supply- Non BAU RPS Qualifying Resources</t>
-  </si>
-  <si>
-    <t>Electricity Supply- Nuclear Plant Lifetime Extension</t>
-  </si>
-  <si>
-    <t>Electricity Supply- Reduce Soft Costs</t>
-  </si>
-  <si>
-    <t>Electricity Supply- Reduce Transmission &amp; Distribution Losses</t>
-  </si>
-  <si>
-    <t>Industry- Cogeneration and Waste Heat Recovery</t>
-  </si>
-  <si>
-    <t>Industry- Early Retirement of Industrial Facilities</t>
-  </si>
-  <si>
-    <t>Industry- Improved System Design</t>
-  </si>
-  <si>
-    <t>Industry- Industry Energy Efficiency Standards</t>
-  </si>
-  <si>
-    <t>Industry- Material Efficiency, Longevity, &amp; Re-Use</t>
-  </si>
-  <si>
-    <t>Industry- Methane Capture</t>
-  </si>
-  <si>
-    <t>Industry- Methane Destruction</t>
-  </si>
-  <si>
-    <t>Industry- Reduce F-gases</t>
-  </si>
-  <si>
-    <t>Industry- Reduce Fossil Fuel Exports</t>
-  </si>
-  <si>
-    <t>Industry- Worker Training</t>
-  </si>
-  <si>
-    <t>Research and Development- Capital Cost Reduction</t>
-  </si>
-  <si>
-    <t>Research and Development- Fuel Use Reduction</t>
-  </si>
-  <si>
-    <t>Transportation- Conventional Pollutant Standards</t>
-  </si>
-  <si>
-    <t>Transportation- Electric Vehicle Charger Deployment</t>
-  </si>
-  <si>
-    <t>Transportation- Electric Vehicle Range &amp; Charging Time</t>
-  </si>
-  <si>
-    <t>Transportation- Electric Vehicle Sales Mandate</t>
-  </si>
-  <si>
-    <t>Transportation- Electric Vehicle Subsidy</t>
-  </si>
-  <si>
-    <t>Transportation- Feebate</t>
-  </si>
-  <si>
-    <t>Transportation- Fuel Economy Standard</t>
-  </si>
-  <si>
-    <t>Transportation- Hydrogen Vehicle Sales Mandate</t>
-  </si>
-  <si>
-    <t>Transportation- Transportation Demand Management</t>
-  </si>
-  <si>
-    <t>Agriculture, Land Use, and Water- Afforestation</t>
-  </si>
-  <si>
-    <t>Agriculture, Land Use, and Water- Avoid Desertification</t>
-  </si>
-  <si>
-    <t>Agriculture, Land Use, and Water- Cropland Management</t>
-  </si>
-  <si>
-    <t>Agriculture, Land Use, and Water- Forest Restoration</t>
-  </si>
-  <si>
-    <t>Agriculture, Land Use, and Water- Forest Set-Asides</t>
-  </si>
-  <si>
-    <t>Agriculture, Land Use, and Water- Improved Forest Management</t>
-  </si>
-  <si>
-    <t>Agriculture, Land Use, and Water- Peatland Restoration</t>
-  </si>
-  <si>
-    <t>Cross-Sector- Carbon Capture, Use, &amp; Sequestration</t>
-  </si>
-  <si>
-    <t>Cross-Sector- End Existing Subsidies</t>
-  </si>
-  <si>
-    <t>Cross-Sector- Fuel Price Deregulation</t>
-  </si>
-  <si>
-    <t>Cross-Sector- Shift Hydrogen Production to Electrolysis</t>
-  </si>
-  <si>
-    <t>Electricity Supply- Carbon-free Electricity Standard</t>
-  </si>
-  <si>
-    <t>Electricity Supply- Non BAU Guaranteed Dispatch</t>
-  </si>
-  <si>
-    <t>Electricity Supply- Subsidy for Electricity Production</t>
-  </si>
-  <si>
-    <t>Industry- Cement Clinker Substitution</t>
-  </si>
-  <si>
-    <t>Industry- Electrification + Hydrogen</t>
-  </si>
-  <si>
-    <t>Transportation- Low Carbon Fuel Standard</t>
-  </si>
-  <si>
-    <t>Cross-Sector- Exempt Non-CO2 Emissions from C Tax</t>
-  </si>
-  <si>
-    <t>Cross-Sector- Exempt Process Emissions from C Tax</t>
-  </si>
-  <si>
-    <t>Cross-Sector- Fixed Energy Prices</t>
-  </si>
-  <si>
-    <t>Electricity Supply- Ban New Power Plants</t>
-  </si>
-  <si>
-    <t>Electricity Supply- Change Electricity Exports</t>
-  </si>
-  <si>
-    <t>Electricity Supply- Change Electricity Imports</t>
-  </si>
-  <si>
-    <t>Electricity Supply- Early Retirement of Power Plants</t>
-  </si>
-  <si>
-    <t>Electricity Supply- Non BAU Mandated Capacity Construction</t>
-  </si>
-  <si>
-    <t>Electricity Supply- Reduce Plant Downtime</t>
+    <t>Agriculture, Land Use, and Water - Desalination Energy Efficiency Standards</t>
+  </si>
+  <si>
+    <t>Agriculture, Land Use, and Water - Livestock Measures</t>
+  </si>
+  <si>
+    <t>Agriculture, Land Use, and Water - Rice Cultivation Measures</t>
+  </si>
+  <si>
+    <t>Agriculture, Land Use, and Water - Shift to Non -Animal Products</t>
+  </si>
+  <si>
+    <t>Agriculture, Land Use, and Water - Water Conservation</t>
+  </si>
+  <si>
+    <t>Buildings and Appliances - Building Component Electrification</t>
+  </si>
+  <si>
+    <t>Buildings and Appliances - Building Energy Efficiency Standards</t>
+  </si>
+  <si>
+    <t>Buildings and Appliances - Contractor Training</t>
+  </si>
+  <si>
+    <t>Buildings and Appliances - Distributed Solar Carve -Out</t>
+  </si>
+  <si>
+    <t>Buildings and Appliances - Distributed Solar Subsidy</t>
+  </si>
+  <si>
+    <t>Buildings and Appliances - Improved Labeling</t>
+  </si>
+  <si>
+    <t>Buildings and Appliances - Rebate for Efficient Products</t>
+  </si>
+  <si>
+    <t>Buildings and Appliances - Retrofit Existing Buildings</t>
+  </si>
+  <si>
+    <t>Cross -Sector - Domestic Carbon Pricing</t>
+  </si>
+  <si>
+    <t>Cross -Sector - Fuel Taxes</t>
+  </si>
+  <si>
+    <t>District Heat and Hydrogen - Switch District Heat Coal to NG</t>
+  </si>
+  <si>
+    <t>District Heat and Hydrogen - Use CHP for District Heat</t>
+  </si>
+  <si>
+    <t>Electricity Supply - Demand Response</t>
+  </si>
+  <si>
+    <t>Electricity Supply - Grid -Scale Electricity Storage</t>
+  </si>
+  <si>
+    <t>Electricity Supply - Increase Transmission</t>
+  </si>
+  <si>
+    <t>Electricity Supply - KSA 2030 Renewables Target</t>
+  </si>
+  <si>
+    <t>Electricity Supply - Non BAU RPS Qualifying Resources</t>
+  </si>
+  <si>
+    <t>Electricity Supply - Nuclear Plant Lifetime Extension</t>
+  </si>
+  <si>
+    <t>Electricity Supply - Reduce Soft Costs</t>
+  </si>
+  <si>
+    <t>Electricity Supply - Reduce Transmission &amp; Distribution Losses</t>
+  </si>
+  <si>
+    <t>Industry - Cogeneration and Waste Heat Recovery</t>
+  </si>
+  <si>
+    <t>Industry - Early Retirement of Industrial Facilities</t>
+  </si>
+  <si>
+    <t>Industry - Improved System Design</t>
+  </si>
+  <si>
+    <t>Industry - Industry Energy Efficiency Standards</t>
+  </si>
+  <si>
+    <t>Industry - Material Efficiency, Longevity, &amp; Re -Use</t>
+  </si>
+  <si>
+    <t>Industry - Methane Capture</t>
+  </si>
+  <si>
+    <t>Industry - Methane Destruction</t>
+  </si>
+  <si>
+    <t>Industry - Reduce F -gases</t>
+  </si>
+  <si>
+    <t>Industry - Reduce Fossil Fuel Exports</t>
+  </si>
+  <si>
+    <t>Industry - Worker Training</t>
+  </si>
+  <si>
+    <t>Research and Development - Capital Cost Reduction</t>
+  </si>
+  <si>
+    <t>Research and Development - Fuel Use Reduction</t>
+  </si>
+  <si>
+    <t>Transportation - Conventional Pollutant Standards</t>
+  </si>
+  <si>
+    <t>Transportation - Electric Vehicle Charger Deployment</t>
+  </si>
+  <si>
+    <t>Transportation - Electric Vehicle Range &amp; Charging Time</t>
+  </si>
+  <si>
+    <t>Transportation - Electric Vehicle Sales Mandate</t>
+  </si>
+  <si>
+    <t>Transportation - Electric Vehicle Subsidy</t>
+  </si>
+  <si>
+    <t>Transportation - Feebate</t>
+  </si>
+  <si>
+    <t>Transportation - Fuel Economy Standard</t>
+  </si>
+  <si>
+    <t>Transportation - Hydrogen Vehicle Sales Mandate</t>
+  </si>
+  <si>
+    <t>Transportation - Transportation Demand Management</t>
+  </si>
+  <si>
+    <t>Agriculture, Land Use, and Water - Afforestation</t>
+  </si>
+  <si>
+    <t>Agriculture, Land Use, and Water - Avoid Desertification</t>
+  </si>
+  <si>
+    <t>Agriculture, Land Use, and Water - Cropland Management</t>
+  </si>
+  <si>
+    <t>Agriculture, Land Use, and Water - Forest Restoration</t>
+  </si>
+  <si>
+    <t>Agriculture, Land Use, and Water - Forest Set -Asides</t>
+  </si>
+  <si>
+    <t>Agriculture, Land Use, and Water - Improved Forest Management</t>
+  </si>
+  <si>
+    <t>Agriculture, Land Use, and Water - Peatland Restoration</t>
+  </si>
+  <si>
+    <t>Cross -Sector - Carbon Capture, Use, &amp; Sequestration</t>
+  </si>
+  <si>
+    <t>Cross -Sector - End Existing Subsidies</t>
+  </si>
+  <si>
+    <t>Cross -Sector - Fuel Price Deregulation</t>
+  </si>
+  <si>
+    <t>Cross -Sector - Shift Hydrogen Production to Electrolysis</t>
+  </si>
+  <si>
+    <t>Electricity Supply - Carbon -free Electricity Standard</t>
+  </si>
+  <si>
+    <t>Electricity Supply - Non BAU Guaranteed Dispatch</t>
+  </si>
+  <si>
+    <t>Electricity Supply - Subsidy for Electricity Production</t>
+  </si>
+  <si>
+    <t>Industry - Cement Clinker Substitution</t>
+  </si>
+  <si>
+    <t>Industry - Electrification + Hydrogen</t>
+  </si>
+  <si>
+    <t>Transportation - Low Carbon Fuel Standard</t>
+  </si>
+  <si>
+    <t>Cross -Sector - Exempt Non -CO2 Emissions from C Tax</t>
+  </si>
+  <si>
+    <t>Cross -Sector - Exempt Process Emissions from C Tax</t>
+  </si>
+  <si>
+    <t>Cross -Sector - Fixed Energy Prices</t>
+  </si>
+  <si>
+    <t>Electricity Supply - Ban New Power Plants</t>
+  </si>
+  <si>
+    <t>Electricity Supply - Change Electricity Exports</t>
+  </si>
+  <si>
+    <t>Electricity Supply - Change Electricity Imports</t>
+  </si>
+  <si>
+    <t>Electricity Supply - Early Retirement of Power Plants</t>
+  </si>
+  <si>
+    <t>Electricity Supply - Non BAU Mandated Capacity Construction</t>
+  </si>
+  <si>
+    <t>Electricity Supply - Reduce Plant Downtime</t>
   </si>
 </sst>
 </file>
@@ -6557,9 +6557,6 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="21" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="21" applyFont="1"/>
     <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -6568,6 +6565,9 @@
     </xf>
     <xf numFmtId="0" fontId="13" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -10998,7 +10998,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B4" sqref="B4"/>
+      <selection pane="bottomLeft" activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.08984375" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -44842,13 +44842,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A1" s="214" t="s">
+      <c r="A1" s="217" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="214"/>
-      <c r="C1" s="214"/>
-      <c r="D1" s="214"/>
-      <c r="E1" s="214"/>
+      <c r="B1" s="217"/>
+      <c r="C1" s="217"/>
+      <c r="D1" s="217"/>
+      <c r="E1" s="217"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="218" t="s">
@@ -44917,13 +44917,13 @@
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A60" s="214" t="s">
+      <c r="A60" s="217" t="s">
         <v>152</v>
       </c>
-      <c r="B60" s="214"/>
-      <c r="C60" s="214"/>
-      <c r="D60" s="214"/>
-      <c r="E60" s="214"/>
+      <c r="B60" s="217"/>
+      <c r="C60" s="217"/>
+      <c r="D60" s="217"/>
+      <c r="E60" s="217"/>
     </row>
     <row r="85" spans="1:39" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A85" s="9" t="s">
@@ -45028,13 +45028,13 @@
       </c>
     </row>
     <row r="89" spans="1:39" x14ac:dyDescent="0.35">
-      <c r="A89" s="214" t="s">
+      <c r="A89" s="217" t="s">
         <v>153</v>
       </c>
-      <c r="B89" s="214"/>
-      <c r="C89" s="214"/>
-      <c r="D89" s="214"/>
-      <c r="E89" s="214"/>
+      <c r="B89" s="217"/>
+      <c r="C89" s="217"/>
+      <c r="D89" s="217"/>
+      <c r="E89" s="217"/>
     </row>
     <row r="90" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A90" s="9">
@@ -45121,13 +45121,13 @@
       </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A98" s="214" t="s">
+      <c r="A98" s="217" t="s">
         <v>154</v>
       </c>
-      <c r="B98" s="214"/>
-      <c r="C98" s="214"/>
-      <c r="D98" s="214"/>
-      <c r="E98" s="214"/>
+      <c r="B98" s="217"/>
+      <c r="C98" s="217"/>
+      <c r="D98" s="217"/>
+      <c r="E98" s="217"/>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A99" s="16">
@@ -45211,13 +45211,13 @@
       <c r="A108" s="19"/>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A109" s="214" t="s">
+      <c r="A109" s="217" t="s">
         <v>156</v>
       </c>
-      <c r="B109" s="214"/>
-      <c r="C109" s="214"/>
-      <c r="D109" s="214"/>
-      <c r="E109" s="214"/>
+      <c r="B109" s="217"/>
+      <c r="C109" s="217"/>
+      <c r="D109" s="217"/>
+      <c r="E109" s="217"/>
     </row>
     <row r="110" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="111" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -45230,13 +45230,13 @@
       </c>
     </row>
     <row r="113" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A113" s="214" t="s">
+      <c r="A113" s="217" t="s">
         <v>155</v>
       </c>
-      <c r="B113" s="214"/>
-      <c r="C113" s="214"/>
-      <c r="D113" s="214"/>
-      <c r="E113" s="214"/>
+      <c r="B113" s="217"/>
+      <c r="C113" s="217"/>
+      <c r="D113" s="217"/>
+      <c r="E113" s="217"/>
     </row>
     <row r="114" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A114" s="16">
@@ -45317,13 +45317,13 @@
       </c>
     </row>
     <row r="124" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A124" s="214" t="s">
+      <c r="A124" s="217" t="s">
         <v>400</v>
       </c>
-      <c r="B124" s="214"/>
-      <c r="C124" s="214"/>
-      <c r="D124" s="214"/>
-      <c r="E124" s="214"/>
+      <c r="B124" s="217"/>
+      <c r="C124" s="217"/>
+      <c r="D124" s="217"/>
+      <c r="E124" s="217"/>
       <c r="L124" s="20"/>
     </row>
     <row r="125" spans="1:14" x14ac:dyDescent="0.35">
@@ -45414,13 +45414,13 @@
       <c r="C133" s="14"/>
     </row>
     <row r="134" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A134" s="214" t="s">
+      <c r="A134" s="217" t="s">
         <v>88</v>
       </c>
-      <c r="B134" s="214"/>
-      <c r="C134" s="214"/>
-      <c r="D134" s="214"/>
-      <c r="E134" s="214"/>
+      <c r="B134" s="217"/>
+      <c r="C134" s="217"/>
+      <c r="D134" s="217"/>
+      <c r="E134" s="217"/>
     </row>
     <row r="135" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A135" s="26" t="s">
@@ -45435,25 +45435,25 @@
     </row>
     <row r="136" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A136" s="28"/>
-      <c r="B136" s="215" t="s">
+      <c r="B136" s="214" t="s">
         <v>420</v>
       </c>
-      <c r="C136" s="216"/>
-      <c r="D136" s="216"/>
-      <c r="E136" s="217"/>
+      <c r="C136" s="215"/>
+      <c r="D136" s="215"/>
+      <c r="E136" s="216"/>
       <c r="F136" s="27"/>
       <c r="G136" s="27"/>
     </row>
     <row r="137" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A137" s="29"/>
-      <c r="B137" s="215" t="s">
+      <c r="B137" s="214" t="s">
         <v>421</v>
       </c>
-      <c r="C137" s="217"/>
-      <c r="D137" s="215" t="s">
+      <c r="C137" s="216"/>
+      <c r="D137" s="214" t="s">
         <v>422</v>
       </c>
-      <c r="E137" s="217"/>
+      <c r="E137" s="216"/>
       <c r="F137" s="27"/>
       <c r="G137" s="27"/>
     </row>
@@ -46000,13 +46000,13 @@
       <c r="G163" s="27"/>
     </row>
     <row r="165" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A165" s="214" t="s">
+      <c r="A165" s="217" t="s">
         <v>159</v>
       </c>
-      <c r="B165" s="214"/>
-      <c r="C165" s="214"/>
-      <c r="D165" s="214"/>
-      <c r="E165" s="214"/>
+      <c r="B165" s="217"/>
+      <c r="C165" s="217"/>
+      <c r="D165" s="217"/>
+      <c r="E165" s="217"/>
     </row>
     <row r="166" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A166" s="22" t="s">
@@ -46029,10 +46029,10 @@
       <c r="B168" s="45"/>
     </row>
     <row r="169" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A169" s="214" t="s">
+      <c r="A169" s="217" t="s">
         <v>408</v>
       </c>
-      <c r="B169" s="214"/>
+      <c r="B169" s="217"/>
     </row>
     <row r="170" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A170" s="22" t="s">
@@ -46064,13 +46064,13 @@
       <c r="B173" s="45"/>
     </row>
     <row r="174" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A174" s="214" t="s">
+      <c r="A174" s="217" t="s">
         <v>168</v>
       </c>
-      <c r="B174" s="214"/>
-      <c r="C174" s="214"/>
-      <c r="D174" s="214"/>
-      <c r="E174" s="214"/>
+      <c r="B174" s="217"/>
+      <c r="C174" s="217"/>
+      <c r="D174" s="217"/>
+      <c r="E174" s="217"/>
     </row>
     <row r="175" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A175" s="22" t="s">
@@ -46090,13 +46090,13 @@
       </c>
     </row>
     <row r="178" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A178" s="214" t="s">
+      <c r="A178" s="217" t="s">
         <v>162</v>
       </c>
-      <c r="B178" s="214"/>
-      <c r="C178" s="214"/>
-      <c r="D178" s="214"/>
-      <c r="E178" s="214"/>
+      <c r="B178" s="217"/>
+      <c r="C178" s="217"/>
+      <c r="D178" s="217"/>
+      <c r="E178" s="217"/>
     </row>
     <row r="179" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A179" s="24" t="s">
@@ -46124,13 +46124,13 @@
       </c>
     </row>
     <row r="183" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A183" s="214" t="s">
+      <c r="A183" s="217" t="s">
         <v>164</v>
       </c>
-      <c r="B183" s="214"/>
-      <c r="C183" s="214"/>
-      <c r="D183" s="214"/>
-      <c r="E183" s="214"/>
+      <c r="B183" s="217"/>
+      <c r="C183" s="217"/>
+      <c r="D183" s="217"/>
+      <c r="E183" s="217"/>
     </row>
     <row r="184" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A184" s="22" t="s">
@@ -46185,13 +46185,13 @@
       </c>
     </row>
     <row r="191" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A191" s="214" t="s">
+      <c r="A191" s="217" t="s">
         <v>178</v>
       </c>
-      <c r="B191" s="214"/>
-      <c r="C191" s="214"/>
-      <c r="D191" s="214"/>
-      <c r="E191" s="214"/>
+      <c r="B191" s="217"/>
+      <c r="C191" s="217"/>
+      <c r="D191" s="217"/>
+      <c r="E191" s="217"/>
     </row>
     <row r="192" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A192" s="20" t="s">
@@ -46251,6 +46251,12 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="A191:E191"/>
+    <mergeCell ref="A165:E165"/>
+    <mergeCell ref="A178:E178"/>
+    <mergeCell ref="A183:E183"/>
+    <mergeCell ref="A174:E174"/>
+    <mergeCell ref="A169:B169"/>
     <mergeCell ref="B136:E136"/>
     <mergeCell ref="B137:C137"/>
     <mergeCell ref="D137:E137"/>
@@ -46265,12 +46271,6 @@
     <mergeCell ref="A113:E113"/>
     <mergeCell ref="A109:E109"/>
     <mergeCell ref="A124:E124"/>
-    <mergeCell ref="A191:E191"/>
-    <mergeCell ref="A165:E165"/>
-    <mergeCell ref="A178:E178"/>
-    <mergeCell ref="A183:E183"/>
-    <mergeCell ref="A174:E174"/>
-    <mergeCell ref="A169:B169"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>